<commit_message>
I'm in love with my creation.
</commit_message>
<xml_diff>
--- a/sql/lebauche.xlsx
+++ b/sql/lebauche.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8952"/>
   </bookViews>
   <sheets>
     <sheet name="geog" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">geog!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">geog!$A$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">hist!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="1035">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -2542,6 +2542,594 @@
   </si>
   <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/thumb/a/a0/Bundesarchiv_Bild_119-1486%2C_Hitler-Putsch%2C_M%C3%BCnchen%2C_Marienplatz.jpg/620px-Bundesarchiv_Bild_119-1486%2C_Hitler-Putsch%2C_M%C3%BCnchen%2C_Marienplatz.jpg</t>
+  </si>
+  <si>
+    <t>capital</t>
+  </si>
+  <si>
+    <t>capitalPic</t>
+  </si>
+  <si>
+    <t>Kabul</t>
+  </si>
+  <si>
+    <t>Tirana</t>
+  </si>
+  <si>
+    <t>Algiers</t>
+  </si>
+  <si>
+    <t>Andorra la Vella</t>
+  </si>
+  <si>
+    <t>Luanda</t>
+  </si>
+  <si>
+    <t>St. John's</t>
+  </si>
+  <si>
+    <t>Buenos Aires</t>
+  </si>
+  <si>
+    <t>Yerevan</t>
+  </si>
+  <si>
+    <t>Canberra</t>
+  </si>
+  <si>
+    <t>Vienna</t>
+  </si>
+  <si>
+    <t>Baku</t>
+  </si>
+  <si>
+    <t>Nassau</t>
+  </si>
+  <si>
+    <t>Manama</t>
+  </si>
+  <si>
+    <t>Dhaka</t>
+  </si>
+  <si>
+    <t>Bridgetown</t>
+  </si>
+  <si>
+    <t>Minsk</t>
+  </si>
+  <si>
+    <t>Brussels</t>
+  </si>
+  <si>
+    <t>Belmopan</t>
+  </si>
+  <si>
+    <t>Porto-Novo</t>
+  </si>
+  <si>
+    <t>Thimphu</t>
+  </si>
+  <si>
+    <t>La Paz</t>
+  </si>
+  <si>
+    <t>Sarajevo</t>
+  </si>
+  <si>
+    <t>Gaborone</t>
+  </si>
+  <si>
+    <t>Brasília</t>
+  </si>
+  <si>
+    <t>Bandar Seri Begawan</t>
+  </si>
+  <si>
+    <t>Sofia</t>
+  </si>
+  <si>
+    <t>Ouagadougou</t>
+  </si>
+  <si>
+    <t>Bujumbura</t>
+  </si>
+  <si>
+    <t>Phnom Penh</t>
+  </si>
+  <si>
+    <t>Yaoundé</t>
+  </si>
+  <si>
+    <t>Ottawa</t>
+  </si>
+  <si>
+    <t>Praia</t>
+  </si>
+  <si>
+    <t>Bangui</t>
+  </si>
+  <si>
+    <t>N'Djamena</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>Bogotá</t>
+  </si>
+  <si>
+    <t>Moroni</t>
+  </si>
+  <si>
+    <t>Brazzaville</t>
+  </si>
+  <si>
+    <t>San José</t>
+  </si>
+  <si>
+    <t>Zagreb</t>
+  </si>
+  <si>
+    <t>Havana</t>
+  </si>
+  <si>
+    <t>Nicosia (south)</t>
+  </si>
+  <si>
+    <t>Prague</t>
+  </si>
+  <si>
+    <t>Yamoussoukro</t>
+  </si>
+  <si>
+    <t>Kinshasa</t>
+  </si>
+  <si>
+    <t>Copenhagen</t>
+  </si>
+  <si>
+    <t>Roseau</t>
+  </si>
+  <si>
+    <t>Santo Domingo</t>
+  </si>
+  <si>
+    <t>Dili</t>
+  </si>
+  <si>
+    <t>Quito</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>San Salvador</t>
+  </si>
+  <si>
+    <t>Malabo</t>
+  </si>
+  <si>
+    <t>Asmara</t>
+  </si>
+  <si>
+    <t>Tallinn</t>
+  </si>
+  <si>
+    <t>Addis Ababa</t>
+  </si>
+  <si>
+    <t>Palikir</t>
+  </si>
+  <si>
+    <t>Suva</t>
+  </si>
+  <si>
+    <t>Helsinki</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Libreville</t>
+  </si>
+  <si>
+    <t>Banjul</t>
+  </si>
+  <si>
+    <t>Tbilisi</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Accra</t>
+  </si>
+  <si>
+    <t>Athens</t>
+  </si>
+  <si>
+    <t>St. George's</t>
+  </si>
+  <si>
+    <t>Guatemala City</t>
+  </si>
+  <si>
+    <t>Conakry</t>
+  </si>
+  <si>
+    <t>Bissau</t>
+  </si>
+  <si>
+    <t>Georgetown</t>
+  </si>
+  <si>
+    <t>Port-au-Prince</t>
+  </si>
+  <si>
+    <t>Tegucigalpa</t>
+  </si>
+  <si>
+    <t>Budapest</t>
+  </si>
+  <si>
+    <t>Reykjavík</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>Tehran</t>
+  </si>
+  <si>
+    <t>Baghdad</t>
+  </si>
+  <si>
+    <t>Dublin</t>
+  </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>Kingston</t>
+  </si>
+  <si>
+    <t>Tokyo</t>
+  </si>
+  <si>
+    <t>Amman</t>
+  </si>
+  <si>
+    <t>Astana</t>
+  </si>
+  <si>
+    <t>Nairobi</t>
+  </si>
+  <si>
+    <t>Tarawa</t>
+  </si>
+  <si>
+    <t>Prishtina</t>
+  </si>
+  <si>
+    <t>Kuwait City</t>
+  </si>
+  <si>
+    <t>Bishkek</t>
+  </si>
+  <si>
+    <t>Vientiane</t>
+  </si>
+  <si>
+    <t>Riga</t>
+  </si>
+  <si>
+    <t>Beirut</t>
+  </si>
+  <si>
+    <t>Maseru</t>
+  </si>
+  <si>
+    <t>Monrovia</t>
+  </si>
+  <si>
+    <t>Tripoli</t>
+  </si>
+  <si>
+    <t>Vaduz</t>
+  </si>
+  <si>
+    <t>Vilnius</t>
+  </si>
+  <si>
+    <t>Skopje</t>
+  </si>
+  <si>
+    <t>Antananarivo</t>
+  </si>
+  <si>
+    <t>Lilongwe</t>
+  </si>
+  <si>
+    <t>Kuala Lumpur</t>
+  </si>
+  <si>
+    <t>Malé</t>
+  </si>
+  <si>
+    <t>Bamako</t>
+  </si>
+  <si>
+    <t>Valletta</t>
+  </si>
+  <si>
+    <t>Majuro</t>
+  </si>
+  <si>
+    <t>Nouakchott</t>
+  </si>
+  <si>
+    <t>Port Louis</t>
+  </si>
+  <si>
+    <t>Mexico City</t>
+  </si>
+  <si>
+    <t>Chişinău</t>
+  </si>
+  <si>
+    <t>Ulaanbaatar</t>
+  </si>
+  <si>
+    <t>Podgorica</t>
+  </si>
+  <si>
+    <t>Rabat</t>
+  </si>
+  <si>
+    <t>Maputo</t>
+  </si>
+  <si>
+    <t>Naypyidaw</t>
+  </si>
+  <si>
+    <t>Windhoek</t>
+  </si>
+  <si>
+    <t>Yaren</t>
+  </si>
+  <si>
+    <t>Kathmandu</t>
+  </si>
+  <si>
+    <t>Amsterdam</t>
+  </si>
+  <si>
+    <t>Wellington</t>
+  </si>
+  <si>
+    <t>Managua</t>
+  </si>
+  <si>
+    <t>Niamey</t>
+  </si>
+  <si>
+    <t>Abuja</t>
+  </si>
+  <si>
+    <t>Pyongyang</t>
+  </si>
+  <si>
+    <t>Oslo</t>
+  </si>
+  <si>
+    <t>Muscat</t>
+  </si>
+  <si>
+    <t>Islamabad</t>
+  </si>
+  <si>
+    <t>Ngerulmud</t>
+  </si>
+  <si>
+    <t>Ramallah</t>
+  </si>
+  <si>
+    <t>Panama City</t>
+  </si>
+  <si>
+    <t>Port Moresby</t>
+  </si>
+  <si>
+    <t>Asunción</t>
+  </si>
+  <si>
+    <t>Lima</t>
+  </si>
+  <si>
+    <t>Manila</t>
+  </si>
+  <si>
+    <t>Warsaw</t>
+  </si>
+  <si>
+    <t>Lisbon</t>
+  </si>
+  <si>
+    <t>Doha</t>
+  </si>
+  <si>
+    <t>Bucharest</t>
+  </si>
+  <si>
+    <t>Moscow</t>
+  </si>
+  <si>
+    <t>Kigali</t>
+  </si>
+  <si>
+    <t>Basseterre</t>
+  </si>
+  <si>
+    <t>Castries</t>
+  </si>
+  <si>
+    <t>Kingstown</t>
+  </si>
+  <si>
+    <t>Apia</t>
+  </si>
+  <si>
+    <t>Riyadh</t>
+  </si>
+  <si>
+    <t>Dakar</t>
+  </si>
+  <si>
+    <t>Belgrade</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>Freetown</t>
+  </si>
+  <si>
+    <t>Bratislava</t>
+  </si>
+  <si>
+    <t>Ljubljana</t>
+  </si>
+  <si>
+    <t>Honiara</t>
+  </si>
+  <si>
+    <t>Mogadishu</t>
+  </si>
+  <si>
+    <t>Pretoria</t>
+  </si>
+  <si>
+    <t>Seoul</t>
+  </si>
+  <si>
+    <t>Juba</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Colombo</t>
+  </si>
+  <si>
+    <t>Khartoum</t>
+  </si>
+  <si>
+    <t>Paramaribo</t>
+  </si>
+  <si>
+    <t>Mbabane</t>
+  </si>
+  <si>
+    <t>Stockholm</t>
+  </si>
+  <si>
+    <t>Bern</t>
+  </si>
+  <si>
+    <t>Damascus</t>
+  </si>
+  <si>
+    <t>São Tomé</t>
+  </si>
+  <si>
+    <t>Dushanbe</t>
+  </si>
+  <si>
+    <t>Dodoma</t>
+  </si>
+  <si>
+    <t>Bangkok</t>
+  </si>
+  <si>
+    <t>Lomé</t>
+  </si>
+  <si>
+    <t>Nukuʻalofa</t>
+  </si>
+  <si>
+    <t>Port of Spain</t>
+  </si>
+  <si>
+    <t>Tunis</t>
+  </si>
+  <si>
+    <t>Ankara</t>
+  </si>
+  <si>
+    <t>Ashgabat</t>
+  </si>
+  <si>
+    <t>Funafuti</t>
+  </si>
+  <si>
+    <t>Kampala</t>
+  </si>
+  <si>
+    <t>Kyiv</t>
+  </si>
+  <si>
+    <t>Abu Dhabi</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Washington, D.C.</t>
+  </si>
+  <si>
+    <t>Montevideo</t>
+  </si>
+  <si>
+    <t>Tashkent</t>
+  </si>
+  <si>
+    <t>Port Vila</t>
+  </si>
+  <si>
+    <t>Caracas</t>
+  </si>
+  <si>
+    <t>Hanoi</t>
+  </si>
+  <si>
+    <t>Sana'a</t>
+  </si>
+  <si>
+    <t>Lusaka</t>
+  </si>
+  <si>
+    <t>Harare</t>
+  </si>
+  <si>
+    <t>Jerusalem (west)</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d5/Presidential_Palace_-_panoramio_%288%29.jpg/298px-Presidential_Palace_-_panoramio_%288%29.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/a/a5/Algiers_Montage.png/550px-Algiers_Montage.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0d/Skanderbeg_square_tirana_2016.jpg/580px-Skanderbeg_square_tirana_2016.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/a/a5/Buenos_Aires_City_Collage.png</t>
   </si>
 </sst>
 </file>
@@ -2875,10 +3463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F197"/>
+  <dimension ref="A1:H197"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F191" sqref="F191"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2889,9 +3477,10 @@
     <col min="4" max="4" width="122.62890625" customWidth="1"/>
     <col min="5" max="5" width="10.62890625" customWidth="1"/>
     <col min="6" max="6" width="14.20703125" customWidth="1"/>
+    <col min="7" max="7" width="11.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>193</v>
       </c>
@@ -2910,8 +3499,14 @@
       <c r="F1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" t="s">
+        <v>839</v>
+      </c>
+      <c r="H1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2930,8 +3525,14 @@
       <c r="F2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" t="s">
+        <v>841</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2950,8 +3551,14 @@
       <c r="F3" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G3" t="s">
+        <v>842</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2970,8 +3577,14 @@
       <c r="F4" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" t="s">
+        <v>843</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2990,8 +3603,11 @@
       <c r="F5" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3010,8 +3626,11 @@
       <c r="F6" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3030,8 +3649,11 @@
       <c r="F7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3050,8 +3672,14 @@
       <c r="F8" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G8" t="s">
+        <v>847</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3070,8 +3698,11 @@
       <c r="F9" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G9" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3090,8 +3721,11 @@
       <c r="F10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G10" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3110,8 +3744,11 @@
       <c r="F11" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G11" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3130,8 +3767,11 @@
       <c r="F12" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G12" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3150,8 +3790,11 @@
       <c r="F13" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G13" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3170,8 +3813,11 @@
       <c r="F14" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G14" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3190,8 +3836,11 @@
       <c r="F15" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G15" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3210,8 +3859,11 @@
       <c r="F16" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G16" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -3230,8 +3882,11 @@
       <c r="F17" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G17" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -3250,8 +3905,11 @@
       <c r="F18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G18" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -3270,8 +3928,11 @@
       <c r="F19" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G19" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -3290,8 +3951,11 @@
       <c r="F20" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G20" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -3310,8 +3974,11 @@
       <c r="F21" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G21" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -3330,8 +3997,11 @@
       <c r="F22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G22" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -3350,8 +4020,11 @@
       <c r="F23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G23" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -3370,8 +4043,11 @@
       <c r="F24" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G24" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -3390,8 +4066,11 @@
       <c r="F25" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G25" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3410,8 +4089,11 @@
       <c r="F26" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G26" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -3430,8 +4112,11 @@
       <c r="F27" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G27" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3450,8 +4135,11 @@
       <c r="F28" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G28" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -3470,8 +4158,11 @@
       <c r="F29" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G29" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -3490,8 +4181,11 @@
       <c r="F30" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G30" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -3510,8 +4204,11 @@
       <c r="F31" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G31" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -3530,8 +4227,11 @@
       <c r="F32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G32" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -3550,8 +4250,11 @@
       <c r="F33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G33" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -3570,8 +4273,11 @@
       <c r="F34" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G34" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -3590,8 +4296,11 @@
       <c r="F35" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G35" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -3610,8 +4319,11 @@
       <c r="F36" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G36" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -3630,8 +4342,11 @@
       <c r="F37" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G37" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -3650,8 +4365,11 @@
       <c r="F38" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G38" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -3670,8 +4388,11 @@
       <c r="F39" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G39" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -3690,8 +4411,11 @@
       <c r="F40" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G40" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -3710,8 +4434,11 @@
       <c r="F41" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G41" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -3730,8 +4457,11 @@
       <c r="F42" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G42" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -3750,8 +4480,11 @@
       <c r="F43" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G43" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -3770,8 +4503,11 @@
       <c r="F44" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G44" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -3790,8 +4526,11 @@
       <c r="F45" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G45" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>255</v>
       </c>
@@ -3810,8 +4549,11 @@
       <c r="F46" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G46" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -3830,8 +4572,11 @@
       <c r="F47" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G47" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -3850,8 +4595,11 @@
       <c r="F48" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -3870,8 +4618,11 @@
       <c r="F49" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G49" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -3890,8 +4641,11 @@
       <c r="F50" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G50" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -3910,8 +4664,11 @@
       <c r="F51" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G51" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -3930,8 +4687,11 @@
       <c r="F52" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G52" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -3950,8 +4710,11 @@
       <c r="F53" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G53" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -3970,8 +4733,11 @@
       <c r="F54" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G54" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -3990,8 +4756,11 @@
       <c r="F55" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G55" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -4010,8 +4779,11 @@
       <c r="F56" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G56" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -4030,8 +4802,11 @@
       <c r="F57" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G57" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -4050,8 +4825,11 @@
       <c r="F58" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G58" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -4070,8 +4848,11 @@
       <c r="F59" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G59" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -4090,8 +4871,11 @@
       <c r="F60" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G60" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -4110,8 +4894,11 @@
       <c r="F61" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G61" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -4130,8 +4917,11 @@
       <c r="F62" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G62" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -4150,8 +4940,11 @@
       <c r="F63" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G63" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -4170,8 +4963,11 @@
       <c r="F64" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G64" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -4190,8 +4986,11 @@
       <c r="F65" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G65" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -4210,8 +5009,11 @@
       <c r="F66" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G66" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -4230,8 +5032,11 @@
       <c r="F67" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G67" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -4250,8 +5055,11 @@
       <c r="F68" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G68" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -4270,8 +5078,11 @@
       <c r="F69" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G69" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -4290,8 +5101,11 @@
       <c r="F70" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G70" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -4310,8 +5124,11 @@
       <c r="F71" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G71" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -4330,8 +5147,11 @@
       <c r="F72" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G72" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -4350,8 +5170,11 @@
       <c r="F73" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G73" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -4370,8 +5193,11 @@
       <c r="F74" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G74" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -4390,8 +5216,11 @@
       <c r="F75" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G75" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -4410,8 +5239,11 @@
       <c r="F76" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G76" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -4430,8 +5262,11 @@
       <c r="F77" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G77" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -4450,8 +5285,11 @@
       <c r="F78" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G78" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -4470,8 +5308,11 @@
       <c r="F79" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G79" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -4490,8 +5331,11 @@
       <c r="F80" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G80" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -4510,8 +5354,11 @@
       <c r="F81" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G81" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -4530,8 +5377,11 @@
       <c r="F82" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G82" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>80</v>
       </c>
@@ -4550,8 +5400,11 @@
       <c r="F83" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G83" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>81</v>
       </c>
@@ -4570,8 +5423,11 @@
       <c r="F84" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G84" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>82</v>
       </c>
@@ -4590,8 +5446,11 @@
       <c r="F85" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G85" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>83</v>
       </c>
@@ -4610,8 +5469,11 @@
       <c r="F86" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G86" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>84</v>
       </c>
@@ -4630,8 +5492,11 @@
       <c r="F87" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G87" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>85</v>
       </c>
@@ -4650,8 +5515,11 @@
       <c r="F88" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G88" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>86</v>
       </c>
@@ -4670,8 +5538,11 @@
       <c r="F89" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G89" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>87</v>
       </c>
@@ -4690,8 +5561,11 @@
       <c r="F90" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G90" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>88</v>
       </c>
@@ -4710,8 +5584,11 @@
       <c r="F91" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G91" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>89</v>
       </c>
@@ -4730,8 +5607,11 @@
       <c r="F92" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G92" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>458</v>
       </c>
@@ -4750,8 +5630,11 @@
       <c r="F93" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G93" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>90</v>
       </c>
@@ -4770,8 +5653,11 @@
       <c r="F94" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G94" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>91</v>
       </c>
@@ -4790,8 +5676,11 @@
       <c r="F95" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G95" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>92</v>
       </c>
@@ -4810,8 +5699,11 @@
       <c r="F96" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G96" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>93</v>
       </c>
@@ -4830,8 +5722,11 @@
       <c r="F97" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G97" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
         <v>94</v>
       </c>
@@ -4850,8 +5745,11 @@
       <c r="F98" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G98" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>95</v>
       </c>
@@ -4870,8 +5768,11 @@
       <c r="F99" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G99" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>96</v>
       </c>
@@ -4890,8 +5791,11 @@
       <c r="F100" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G100" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>97</v>
       </c>
@@ -4910,8 +5814,11 @@
       <c r="F101" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G101" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
         <v>98</v>
       </c>
@@ -4930,8 +5837,11 @@
       <c r="F102" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G102" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
         <v>99</v>
       </c>
@@ -4950,8 +5860,11 @@
       <c r="F103" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G103" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
         <v>100</v>
       </c>
@@ -4970,8 +5883,11 @@
       <c r="F104" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G104" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>253</v>
       </c>
@@ -4990,8 +5906,11 @@
       <c r="F105" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G105" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
         <v>101</v>
       </c>
@@ -5010,8 +5929,11 @@
       <c r="F106" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G106" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
         <v>102</v>
       </c>
@@ -5030,8 +5952,11 @@
       <c r="F107" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G107" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
         <v>103</v>
       </c>
@@ -5050,8 +5975,11 @@
       <c r="F108" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G108" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
         <v>104</v>
       </c>
@@ -5070,8 +5998,11 @@
       <c r="F109" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G109" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
         <v>105</v>
       </c>
@@ -5090,8 +6021,11 @@
       <c r="F110" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G110" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
         <v>106</v>
       </c>
@@ -5110,8 +6044,11 @@
       <c r="F111" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G111" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
         <v>107</v>
       </c>
@@ -5130,8 +6067,11 @@
       <c r="F112" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G112" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
         <v>108</v>
       </c>
@@ -5150,8 +6090,11 @@
       <c r="F113" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G113" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
         <v>109</v>
       </c>
@@ -5170,8 +6113,11 @@
       <c r="F114" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G114" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
         <v>110</v>
       </c>
@@ -5190,8 +6136,11 @@
       <c r="F115" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G115" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
         <v>111</v>
       </c>
@@ -5210,8 +6159,11 @@
       <c r="F116" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G116" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
         <v>112</v>
       </c>
@@ -5230,8 +6182,11 @@
       <c r="F117" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G117" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
         <v>113</v>
       </c>
@@ -5250,8 +6205,11 @@
       <c r="F118" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G118" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
         <v>114</v>
       </c>
@@ -5270,8 +6228,11 @@
       <c r="F119" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G119" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
         <v>115</v>
       </c>
@@ -5290,8 +6251,11 @@
       <c r="F120" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G120" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
         <v>116</v>
       </c>
@@ -5310,8 +6274,11 @@
       <c r="F121" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G121" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
         <v>117</v>
       </c>
@@ -5330,8 +6297,11 @@
       <c r="F122" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G122" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
         <v>118</v>
       </c>
@@ -5350,8 +6320,11 @@
       <c r="F123" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G123" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
         <v>119</v>
       </c>
@@ -5370,8 +6343,11 @@
       <c r="F124" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G124" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
         <v>120</v>
       </c>
@@ -5390,8 +6366,11 @@
       <c r="F125" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G125" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
         <v>121</v>
       </c>
@@ -5410,8 +6389,11 @@
       <c r="F126" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G126" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
         <v>122</v>
       </c>
@@ -5430,8 +6412,11 @@
       <c r="F127" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G127" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
         <v>123</v>
       </c>
@@ -5450,8 +6435,11 @@
       <c r="F128" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G128" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
         <v>124</v>
       </c>
@@ -5470,8 +6458,11 @@
       <c r="F129" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G129" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
         <v>125</v>
       </c>
@@ -5490,8 +6481,11 @@
       <c r="F130" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G130" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
         <v>126</v>
       </c>
@@ -5510,8 +6504,11 @@
       <c r="F131" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G131" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
         <v>127</v>
       </c>
@@ -5530,8 +6527,11 @@
       <c r="F132" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G132" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
         <v>128</v>
       </c>
@@ -5550,8 +6550,11 @@
       <c r="F133" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G133" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
         <v>129</v>
       </c>
@@ -5570,8 +6573,11 @@
       <c r="F134" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G134" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
         <v>130</v>
       </c>
@@ -5590,8 +6596,11 @@
       <c r="F135" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G135" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
         <v>131</v>
       </c>
@@ -5610,8 +6619,11 @@
       <c r="F136" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G136" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
         <v>132</v>
       </c>
@@ -5630,8 +6642,11 @@
       <c r="F137" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G137" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" t="s">
         <v>133</v>
       </c>
@@ -5650,8 +6665,11 @@
       <c r="F138" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G138" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" t="s">
         <v>134</v>
       </c>
@@ -5670,8 +6688,11 @@
       <c r="F139" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G139" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" t="s">
         <v>135</v>
       </c>
@@ -5690,8 +6711,11 @@
       <c r="F140" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G140" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" t="s">
         <v>136</v>
       </c>
@@ -5710,8 +6734,11 @@
       <c r="F141" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G141" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" t="s">
         <v>137</v>
       </c>
@@ -5730,8 +6757,11 @@
       <c r="F142" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G142" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" t="s">
         <v>138</v>
       </c>
@@ -5750,8 +6780,11 @@
       <c r="F143" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G143" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" t="s">
         <v>139</v>
       </c>
@@ -5770,8 +6803,11 @@
       <c r="F144" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G144" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" t="s">
         <v>140</v>
       </c>
@@ -5790,8 +6826,11 @@
       <c r="F145" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G145" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" t="s">
         <v>141</v>
       </c>
@@ -5810,8 +6849,11 @@
       <c r="F146" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G146" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
         <v>142</v>
       </c>
@@ -5830,8 +6872,11 @@
       <c r="F147" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G147" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" t="s">
         <v>143</v>
       </c>
@@ -5850,8 +6895,11 @@
       <c r="F148" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G148" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
         <v>144</v>
       </c>
@@ -5870,8 +6918,11 @@
       <c r="F149" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G149" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="s">
         <v>145</v>
       </c>
@@ -5890,8 +6941,11 @@
       <c r="F150" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G150" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="s">
         <v>146</v>
       </c>
@@ -5910,8 +6964,11 @@
       <c r="F151" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G151" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" t="s">
         <v>147</v>
       </c>
@@ -5930,8 +6987,11 @@
       <c r="F152" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G152" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
         <v>148</v>
       </c>
@@ -5950,8 +7010,11 @@
       <c r="F153" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G153" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
         <v>149</v>
       </c>
@@ -5970,8 +7033,11 @@
       <c r="F154" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G154" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
         <v>150</v>
       </c>
@@ -5990,8 +7056,11 @@
       <c r="F155" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G155" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
         <v>151</v>
       </c>
@@ -6010,8 +7079,11 @@
       <c r="F156" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G156" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="s">
         <v>152</v>
       </c>
@@ -6030,8 +7102,11 @@
       <c r="F157" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G157" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
         <v>153</v>
       </c>
@@ -6050,8 +7125,11 @@
       <c r="F158" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G158" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" t="s">
         <v>154</v>
       </c>
@@ -6070,8 +7148,11 @@
       <c r="F159" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G159" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="s">
         <v>155</v>
       </c>
@@ -6090,8 +7171,11 @@
       <c r="F160" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G160" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" t="s">
         <v>156</v>
       </c>
@@ -6110,8 +7194,11 @@
       <c r="F161" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G161" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" t="s">
         <v>157</v>
       </c>
@@ -6130,8 +7217,11 @@
       <c r="F162" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G162" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" t="s">
         <v>158</v>
       </c>
@@ -6150,8 +7240,11 @@
       <c r="F163" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G163" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" t="s">
         <v>159</v>
       </c>
@@ -6170,8 +7263,11 @@
       <c r="F164" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G164" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" t="s">
         <v>160</v>
       </c>
@@ -6190,8 +7286,11 @@
       <c r="F165" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G165" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="s">
         <v>161</v>
       </c>
@@ -6210,8 +7309,11 @@
       <c r="F166" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G166" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" t="s">
         <v>162</v>
       </c>
@@ -6230,8 +7332,11 @@
       <c r="F167" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G167" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" t="s">
         <v>163</v>
       </c>
@@ -6250,8 +7355,11 @@
       <c r="F168" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G168" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" t="s">
         <v>164</v>
       </c>
@@ -6270,8 +7378,11 @@
       <c r="F169" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G169" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" t="s">
         <v>165</v>
       </c>
@@ -6290,8 +7401,11 @@
       <c r="F170" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G170" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="s">
         <v>166</v>
       </c>
@@ -6310,8 +7424,11 @@
       <c r="F171" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G171" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" t="s">
         <v>167</v>
       </c>
@@ -6330,8 +7447,11 @@
       <c r="F172" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G172" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
         <v>168</v>
       </c>
@@ -6350,8 +7470,11 @@
       <c r="F173" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G173" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
         <v>169</v>
       </c>
@@ -6370,8 +7493,11 @@
       <c r="F174" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G174" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
         <v>170</v>
       </c>
@@ -6390,8 +7516,11 @@
       <c r="F175" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G175" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" t="s">
         <v>171</v>
       </c>
@@ -6410,8 +7539,11 @@
       <c r="F176" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G176" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="s">
         <v>172</v>
       </c>
@@ -6430,8 +7562,11 @@
       <c r="F177" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G177" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" t="s">
         <v>173</v>
       </c>
@@ -6450,8 +7585,11 @@
       <c r="F178" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G178" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" t="s">
         <v>174</v>
       </c>
@@ -6470,8 +7608,11 @@
       <c r="F179" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G179" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="s">
         <v>175</v>
       </c>
@@ -6490,8 +7631,11 @@
       <c r="F180" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G180" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" t="s">
         <v>176</v>
       </c>
@@ -6510,8 +7654,11 @@
       <c r="F181" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G181" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" t="s">
         <v>177</v>
       </c>
@@ -6530,8 +7677,11 @@
       <c r="F182" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G182" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" t="s">
         <v>178</v>
       </c>
@@ -6550,8 +7700,11 @@
       <c r="F183" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G183" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="s">
         <v>179</v>
       </c>
@@ -6570,8 +7723,11 @@
       <c r="F184" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G184" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
         <v>180</v>
       </c>
@@ -6590,8 +7746,11 @@
       <c r="F185" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G185" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="s">
         <v>181</v>
       </c>
@@ -6610,8 +7769,11 @@
       <c r="F186" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G186" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" t="s">
         <v>182</v>
       </c>
@@ -6630,8 +7792,11 @@
       <c r="F187" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G187" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" t="s">
         <v>183</v>
       </c>
@@ -6650,8 +7815,11 @@
       <c r="F188" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G188" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" t="s">
         <v>184</v>
       </c>
@@ -6670,8 +7838,11 @@
       <c r="F189" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G189" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" t="s">
         <v>185</v>
       </c>
@@ -6690,8 +7861,11 @@
       <c r="F190" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G190" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" t="s">
         <v>186</v>
       </c>
@@ -6710,8 +7884,11 @@
       <c r="F191" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G191" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" t="s">
         <v>187</v>
       </c>
@@ -6730,8 +7907,11 @@
       <c r="F192" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G192" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" t="s">
         <v>188</v>
       </c>
@@ -6750,8 +7930,11 @@
       <c r="F193" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G193" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" t="s">
         <v>189</v>
       </c>
@@ -6770,8 +7953,11 @@
       <c r="F194" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G194" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" t="s">
         <v>190</v>
       </c>
@@ -6790,8 +7976,11 @@
       <c r="F195" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G195" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" t="s">
         <v>191</v>
       </c>
@@ -6810,8 +7999,11 @@
       <c r="F196" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G196" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" t="s">
         <v>192</v>
       </c>
@@ -6830,9 +8022,12 @@
       <c r="F197" t="s">
         <v>179</v>
       </c>
+      <c r="G197" t="s">
+        <v>1029</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:H1"/>
   <hyperlinks>
     <hyperlink ref="C30" r:id="rId1"/>
     <hyperlink ref="C36" r:id="rId2"/>
@@ -7029,6 +8224,9 @@
     <hyperlink ref="C151" r:id="rId193"/>
     <hyperlink ref="C174" r:id="rId194"/>
     <hyperlink ref="C183" r:id="rId195"/>
+    <hyperlink ref="H2" r:id="rId196"/>
+    <hyperlink ref="H4" r:id="rId197"/>
+    <hyperlink ref="H8" r:id="rId198"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7038,7 +8236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>

</xml_diff>